<commit_message>
Super Model - 50epoch 번역 테스트
</commit_message>
<xml_diff>
--- a/Super Model/SuperModel_Result.xlsx
+++ b/Super Model/SuperModel_Result.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahjeong_park/Study/Attention-Ensemble-Translation/Super Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B6F6C5-BE13-544E-9F63-3DFB8109810F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D301471-C91A-A841-963D-F23C0F5E7C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-4800" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuperModel" sheetId="1" r:id="rId1"/>
+    <sheet name="SuperModel(2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="246">
   <si>
     <t>문장</t>
   </si>
@@ -308,13 +309,468 @@
   </si>
   <si>
     <t xml:space="preserve">how old she first drove a car ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Te dijeron lo que pasó, ¿no?</t>
+  </si>
+  <si>
+    <t>They told you what happened, didn't they?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">you ve told you what happened ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Ellos no estaban allá.</t>
+  </si>
+  <si>
+    <t>They weren't there.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">they aren t there . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>No me gusta ninguno de los chicos.</t>
+  </si>
+  <si>
+    <t>I don't like either of the boys.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i don t like any of them . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Jamás trabajé con él.</t>
+  </si>
+  <si>
+    <t>I never worked with him.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i never worked with him . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Mi padre cultiva arroz.</t>
+  </si>
+  <si>
+    <t>My father grows rice.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my father has allergies need . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Dime qué hiciste en Shounan.</t>
+  </si>
+  <si>
+    <t>Tell me what you did in Shounan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tell me you did anything . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Cuántas palabras deberías escribir?</t>
+  </si>
+  <si>
+    <t>How many words should you write?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how many your words should write ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Cómo te introdujiste en mi casa?</t>
+  </si>
+  <si>
+    <t>How did you get in my house?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how often do you in my house ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Mi madre hornea pan todas las mañanas.</t>
+  </si>
+  <si>
+    <t>My mother bakes bread every morning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my mother bakes bread every morning . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Yo he disfrutado el leer esta novela.</t>
+  </si>
+  <si>
+    <t>I have enjoyed reading this novel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i enjoyed the novel is novel . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Él estaba parado en la esquina.</t>
+  </si>
+  <si>
+    <t>He was standing at the street corner.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">he was standing on the corner . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>El testigo no parecía estar nervioso cuando testificó en el juicio.</t>
+  </si>
+  <si>
+    <t>The witness did not seem nervous when he spoke at the trial.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the battery never promised to be nervous when kept getting kept on his feet . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Dónde está el zoológico?</t>
+  </si>
+  <si>
+    <t>Where's the zoo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">where is the zoo ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>El nombre de mi hijo es Tom.</t>
+  </si>
+  <si>
+    <t>My son's name is Tom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my name of my son is tom . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Tenemos cosas más grandes de qué preocuparnos.</t>
+  </si>
+  <si>
+    <t>We have bigger things to worry about.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we have some more than to worry about . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Juntémonos pasado mañana.</t>
+  </si>
+  <si>
+    <t>Let's meet the day after tomorrow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">let s get together till tomorrow . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Qué estás escribiendo?</t>
+  </si>
+  <si>
+    <t>What are you writing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what re you writing ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Este es tu vino?</t>
+  </si>
+  <si>
+    <t>Is this your wine?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is this your wine ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Era casi imposible circular por esa calle.</t>
+  </si>
+  <si>
+    <t>It was almost impossible to get around on that street.</t>
+  </si>
+  <si>
+    <t>no word</t>
+  </si>
+  <si>
+    <t>Pensé que Tom querría ayudarme.</t>
+  </si>
+  <si>
+    <t>I thought Tom would want to help me.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i thought tom would want to help me . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Qué le quieres regalar a Tom?</t>
+  </si>
+  <si>
+    <t>What do you want to give Tom?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what do you want to give tom up ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>No quiero permitir que eso suceda.</t>
+  </si>
+  <si>
+    <t>I don't want to let that happen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i don t want to be saying that to happen . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>No queda rollo de papel.</t>
+  </si>
+  <si>
+    <t>There's no toilet paper.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no food left paper . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Vas a venir a visitarme?</t>
+  </si>
+  <si>
+    <t>Are you going to come visit me?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">are you going along ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Asumo que estás aquí para preguntarme por Tom.</t>
+  </si>
+  <si>
+    <t>I assume you're here to ask me about Tom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i assume you re here for me for tom . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Tom le apreció a Mary su bondad.</t>
+  </si>
+  <si>
+    <t>Tom appreciated Mary's kindness.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tom appreciated mary s kindness . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Dónde está la otra?</t>
+  </si>
+  <si>
+    <t>Where's the other one?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">where s the other ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Los pobres no siempre son infelices.</t>
+  </si>
+  <si>
+    <t>The poor are not always unhappy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the poor aren t always dead . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>La perseverancia, como usted sabe, es la llave al éxito.</t>
+  </si>
+  <si>
+    <t>Perseverance, as you know, is the key to success.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">over , you know , she is the key to the success . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Tom aparece a veces en la televisión.</t>
+  </si>
+  <si>
+    <t>Tom sometimes appears on TV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tom respected that in the tv . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Me gusta el perro.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i like the dog . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Es algo que tengo que hacer.</t>
+  </si>
+  <si>
+    <t>It's something I have to do.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is something i have to do . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Tom no era muy bueno para leer entre líneas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tom was not very good at reading . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Podrías venir acá?</t>
+  </si>
+  <si>
+    <t>Would you please come over here?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">would you please come over here ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Esa racha de suerte no durará para siempre.</t>
+  </si>
+  <si>
+    <t>This run of good luck won't last forever.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this lucky streak won t last forever . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Caminaste todo el camino hasta acá?</t>
+  </si>
+  <si>
+    <t>Did you walk all the way here?</t>
+  </si>
+  <si>
+    <t>Pensé que Tom había dejado a Mary hace un mes.</t>
+  </si>
+  <si>
+    <t>I thought Tom dumped Mary a month ago.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i thought tom had stopped mary a month ago . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Dibuja una línea en el folio.</t>
+  </si>
+  <si>
+    <t>Draw a line on the paper.</t>
+  </si>
+  <si>
+    <t>La fogata sigue encendida.</t>
+  </si>
+  <si>
+    <t>The campfire is still burning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the administration is on inside . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Es cruel burlarse de un ciego.</t>
+  </si>
+  <si>
+    <t>It is cruel to mock a blind man.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it s cruel to get hurt water . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¡Qué hermoso regalo!</t>
+  </si>
+  <si>
+    <t>What a wonderful gift!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what a wonderful present ! &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Actualmente, Tom no tiene empleo.</t>
+  </si>
+  <si>
+    <t>Tom currently doesn't have a job.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tom currently doesn t have a job . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>La ciudad estaba envuelta en niebla.</t>
+  </si>
+  <si>
+    <t>The city was wrapped in fog.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the city was enveloped in fog . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Sabes cómo usar esto?</t>
+  </si>
+  <si>
+    <t>Do you know how to use this?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do you know how to use this ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Tom cenó hace más o menos una hora.</t>
+  </si>
+  <si>
+    <t>Tom ate dinner about one hour ago.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tom had a longer if he called an hour . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>¿Podrías darme tu nombre y tu número de teléfono?</t>
+  </si>
+  <si>
+    <t>Would you tell me your name and phone number?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">could you give me your name and telephone number ? &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Los documentos secretos fueron triturados.</t>
+  </si>
+  <si>
+    <t>The secret documents were shredded.</t>
+  </si>
+  <si>
+    <t>Tom está en una racha de suerte.</t>
+  </si>
+  <si>
+    <t>Tom is on a winning streak.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tom is on a winning streak . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>El enemigo más terrible es un amigo pasado.</t>
+  </si>
+  <si>
+    <t>The most terrible enemy is a former friend.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the enemy other for is a nice friend . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>Tom es un conductor muy precavido.</t>
+  </si>
+  <si>
+    <t>Tom is a very careful driver.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tom is a very talented end . &lt;end&gt; </t>
+  </si>
+  <si>
+    <t>번역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I like the dog.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom wasn't very good at reading between the lines.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuperModel 결과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -325,6 +781,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -386,7 +850,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -405,12 +869,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,12 +888,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFE98386"/>
-      <color rgb="FFE95E8E"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -735,15 +1199,15 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J162" sqref="J162"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48" style="6" customWidth="1"/>
+    <col min="3" max="3" width="48" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -764,21 +1228,21 @@
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3"/>
+      <c r="A3" s="8"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4"/>
+      <c r="A4" s="8"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5"/>
+      <c r="A5" s="8"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6"/>
+      <c r="A6" s="8"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4"/>
@@ -790,7 +1254,7 @@
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -801,7 +1265,7 @@
       <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -812,7 +1276,7 @@
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -823,7 +1287,7 @@
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -834,7 +1298,7 @@
       <c r="B32" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -845,7 +1309,7 @@
       <c r="B38" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -856,7 +1320,7 @@
       <c r="B44" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -867,7 +1331,7 @@
       <c r="B50" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -878,7 +1342,7 @@
       <c r="B56" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -889,7 +1353,7 @@
       <c r="B62" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -900,7 +1364,7 @@
       <c r="B68" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -922,7 +1386,7 @@
       <c r="B80" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -933,7 +1397,7 @@
       <c r="B86" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -944,7 +1408,7 @@
       <c r="B92" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -955,7 +1419,7 @@
       <c r="B98" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C98" s="6" t="s">
         <v>53</v>
       </c>
     </row>
@@ -966,7 +1430,7 @@
       <c r="B104" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C104" s="6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -977,7 +1441,7 @@
       <c r="B110" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -988,7 +1452,7 @@
       <c r="B116" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="8" t="s">
         <v>62</v>
       </c>
     </row>
@@ -999,7 +1463,7 @@
       <c r="B122" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="8" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1010,7 +1474,7 @@
       <c r="B128" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="8" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1021,7 +1485,7 @@
       <c r="B134" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C134" s="7" t="s">
+      <c r="C134" s="6" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1032,7 +1496,7 @@
       <c r="B140" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C140" s="7" t="s">
+      <c r="C140" s="6" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1043,7 +1507,7 @@
       <c r="B146" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C146" s="7" t="s">
+      <c r="C146" s="6" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1054,7 +1518,7 @@
       <c r="B152" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C152" s="7" t="s">
+      <c r="C152" s="6" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1065,7 +1529,7 @@
       <c r="B158" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C158" s="7" t="s">
+      <c r="C158" s="6" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1076,7 +1540,7 @@
       <c r="B164" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C164" s="7" t="s">
+      <c r="C164" s="6" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1087,7 +1551,7 @@
       <c r="B170" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C170" s="8" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1098,7 +1562,7 @@
       <c r="B176" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C176" s="8" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1109,9 +1573,1105 @@
       <c r="B182" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="8" t="s">
         <v>95</v>
       </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C430"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="9"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="9"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="19" customHeight="1">
+      <c r="A8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C146" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C182" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="3"/>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C188" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="9"/>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="9"/>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="9"/>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="9"/>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="4"/>
+      <c r="B193" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C194" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="3"/>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C200" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="3"/>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C206" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="3"/>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C212" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="3"/>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C218" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C224" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C230" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C236" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C242" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C248" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C254" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C260" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C266" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B272" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C272" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B278" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C278" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C284" s="8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C290" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B296" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C296" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="B297" s="9"/>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="B298" s="9"/>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="B299" s="9"/>
+    </row>
+    <row r="300" spans="1:3">
+      <c r="B300" s="9"/>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="B301" s="7"/>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="B302" s="9"/>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="B303" s="9"/>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="B304" s="9"/>
+    </row>
+    <row r="305" spans="2:2">
+      <c r="B305" s="9"/>
+    </row>
+    <row r="306" spans="2:2">
+      <c r="B306" s="9"/>
+    </row>
+    <row r="307" spans="2:2">
+      <c r="B307" s="7"/>
+    </row>
+    <row r="308" spans="2:2">
+      <c r="B308" s="9"/>
+    </row>
+    <row r="309" spans="2:2">
+      <c r="B309" s="9"/>
+    </row>
+    <row r="310" spans="2:2">
+      <c r="B310" s="9"/>
+    </row>
+    <row r="311" spans="2:2">
+      <c r="B311" s="9"/>
+    </row>
+    <row r="312" spans="2:2">
+      <c r="B312" s="9"/>
+    </row>
+    <row r="313" spans="2:2">
+      <c r="B313" s="7"/>
+    </row>
+    <row r="314" spans="2:2">
+      <c r="B314" s="9"/>
+    </row>
+    <row r="315" spans="2:2">
+      <c r="B315" s="9"/>
+    </row>
+    <row r="316" spans="2:2">
+      <c r="B316" s="9"/>
+    </row>
+    <row r="317" spans="2:2">
+      <c r="B317" s="9"/>
+    </row>
+    <row r="318" spans="2:2">
+      <c r="B318" s="9"/>
+    </row>
+    <row r="319" spans="2:2">
+      <c r="B319" s="7"/>
+    </row>
+    <row r="320" spans="2:2">
+      <c r="B320" s="9"/>
+    </row>
+    <row r="321" spans="1:2">
+      <c r="A321" s="10"/>
+      <c r="B321" s="9"/>
+    </row>
+    <row r="322" spans="1:2">
+      <c r="B322" s="9"/>
+    </row>
+    <row r="323" spans="1:2">
+      <c r="B323" s="9"/>
+    </row>
+    <row r="324" spans="1:2">
+      <c r="B324" s="9"/>
+    </row>
+    <row r="325" spans="1:2">
+      <c r="B325" s="7"/>
+    </row>
+    <row r="326" spans="1:2">
+      <c r="B326" s="9"/>
+    </row>
+    <row r="327" spans="1:2">
+      <c r="B327" s="9"/>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="B328" s="9"/>
+    </row>
+    <row r="329" spans="1:2">
+      <c r="B329" s="9"/>
+    </row>
+    <row r="330" spans="1:2">
+      <c r="B330" s="9"/>
+    </row>
+    <row r="331" spans="1:2">
+      <c r="B331" s="7"/>
+    </row>
+    <row r="332" spans="1:2">
+      <c r="B332" s="9"/>
+    </row>
+    <row r="333" spans="1:2">
+      <c r="B333" s="9"/>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="B334" s="9"/>
+    </row>
+    <row r="335" spans="1:2">
+      <c r="B335" s="9"/>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="B336" s="9"/>
+    </row>
+    <row r="337" spans="2:2">
+      <c r="B337" s="7"/>
+    </row>
+    <row r="338" spans="2:2">
+      <c r="B338" s="9"/>
+    </row>
+    <row r="339" spans="2:2">
+      <c r="B339" s="9"/>
+    </row>
+    <row r="340" spans="2:2">
+      <c r="B340" s="9"/>
+    </row>
+    <row r="341" spans="2:2">
+      <c r="B341" s="9"/>
+    </row>
+    <row r="342" spans="2:2">
+      <c r="B342" s="9"/>
+    </row>
+    <row r="343" spans="2:2">
+      <c r="B343" s="7"/>
+    </row>
+    <row r="344" spans="2:2">
+      <c r="B344" s="9"/>
+    </row>
+    <row r="345" spans="2:2">
+      <c r="B345" s="9"/>
+    </row>
+    <row r="346" spans="2:2">
+      <c r="B346" s="9"/>
+    </row>
+    <row r="347" spans="2:2">
+      <c r="B347" s="9"/>
+    </row>
+    <row r="348" spans="2:2">
+      <c r="B348" s="9"/>
+    </row>
+    <row r="349" spans="2:2">
+      <c r="B349" s="7"/>
+    </row>
+    <row r="350" spans="2:2">
+      <c r="B350" s="9"/>
+    </row>
+    <row r="351" spans="2:2">
+      <c r="B351" s="9"/>
+    </row>
+    <row r="352" spans="2:2">
+      <c r="B352" s="9"/>
+    </row>
+    <row r="353" spans="1:2">
+      <c r="B353" s="9"/>
+    </row>
+    <row r="354" spans="1:2">
+      <c r="B354" s="9"/>
+    </row>
+    <row r="355" spans="1:2">
+      <c r="B355" s="7"/>
+    </row>
+    <row r="356" spans="1:2">
+      <c r="B356" s="9"/>
+    </row>
+    <row r="357" spans="1:2">
+      <c r="B357" s="9"/>
+    </row>
+    <row r="358" spans="1:2">
+      <c r="B358" s="9"/>
+    </row>
+    <row r="359" spans="1:2">
+      <c r="B359" s="9"/>
+    </row>
+    <row r="360" spans="1:2">
+      <c r="A360" s="10"/>
+      <c r="B360" s="9"/>
+    </row>
+    <row r="361" spans="1:2">
+      <c r="B361" s="7"/>
+    </row>
+    <row r="362" spans="1:2">
+      <c r="B362" s="9"/>
+    </row>
+    <row r="363" spans="1:2">
+      <c r="B363" s="9"/>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="B364" s="9"/>
+    </row>
+    <row r="365" spans="1:2">
+      <c r="B365" s="9"/>
+    </row>
+    <row r="366" spans="1:2">
+      <c r="B366" s="9"/>
+    </row>
+    <row r="367" spans="1:2">
+      <c r="B367" s="7"/>
+    </row>
+    <row r="368" spans="1:2">
+      <c r="B368" s="9"/>
+    </row>
+    <row r="369" spans="1:2">
+      <c r="A369" s="9"/>
+      <c r="B369" s="9"/>
+    </row>
+    <row r="370" spans="1:2">
+      <c r="A370" s="9"/>
+      <c r="B370" s="9"/>
+    </row>
+    <row r="371" spans="1:2">
+      <c r="A371" s="9"/>
+      <c r="B371" s="9"/>
+    </row>
+    <row r="372" spans="1:2">
+      <c r="A372" s="9"/>
+      <c r="B372" s="9"/>
+    </row>
+    <row r="373" spans="1:2">
+      <c r="A373" s="7"/>
+      <c r="B373" s="7"/>
+    </row>
+    <row r="374" spans="1:2">
+      <c r="A374" s="7"/>
+      <c r="B374" s="7"/>
+    </row>
+    <row r="375" spans="1:2">
+      <c r="A375" s="7"/>
+      <c r="B375" s="7"/>
+    </row>
+    <row r="376" spans="1:2">
+      <c r="A376" s="7"/>
+      <c r="B376" s="7"/>
+    </row>
+    <row r="377" spans="1:2">
+      <c r="A377" s="7"/>
+      <c r="B377" s="7"/>
+    </row>
+    <row r="378" spans="1:2">
+      <c r="A378" s="7"/>
+      <c r="B378" s="7"/>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="A379" s="7"/>
+      <c r="B379" s="7"/>
+    </row>
+    <row r="380" spans="1:2">
+      <c r="A380" s="7"/>
+      <c r="B380" s="7"/>
+    </row>
+    <row r="381" spans="1:2">
+      <c r="A381" s="7"/>
+      <c r="B381" s="7"/>
+    </row>
+    <row r="382" spans="1:2">
+      <c r="A382" s="7"/>
+      <c r="B382" s="7"/>
+    </row>
+    <row r="383" spans="1:2">
+      <c r="A383" s="7"/>
+      <c r="B383" s="7"/>
+    </row>
+    <row r="384" spans="1:2">
+      <c r="A384" s="7"/>
+      <c r="B384" s="7"/>
+    </row>
+    <row r="385" spans="1:2">
+      <c r="A385" s="7"/>
+      <c r="B385" s="7"/>
+    </row>
+    <row r="386" spans="1:2">
+      <c r="A386" s="7"/>
+      <c r="B386" s="7"/>
+    </row>
+    <row r="387" spans="1:2">
+      <c r="A387" s="7"/>
+      <c r="B387" s="7"/>
+    </row>
+    <row r="388" spans="1:2">
+      <c r="A388" s="7"/>
+      <c r="B388" s="7"/>
+    </row>
+    <row r="389" spans="1:2">
+      <c r="A389" s="7"/>
+      <c r="B389" s="7"/>
+    </row>
+    <row r="390" spans="1:2">
+      <c r="A390" s="7"/>
+      <c r="B390" s="7"/>
+    </row>
+    <row r="391" spans="1:2">
+      <c r="A391" s="7"/>
+      <c r="B391" s="7"/>
+    </row>
+    <row r="392" spans="1:2">
+      <c r="A392" s="7"/>
+      <c r="B392" s="7"/>
+    </row>
+    <row r="393" spans="1:2">
+      <c r="A393" s="7"/>
+      <c r="B393" s="7"/>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="A394" s="7"/>
+      <c r="B394" s="7"/>
+    </row>
+    <row r="395" spans="1:2">
+      <c r="A395" s="7"/>
+      <c r="B395" s="7"/>
+    </row>
+    <row r="396" spans="1:2">
+      <c r="A396" s="7"/>
+      <c r="B396" s="7"/>
+    </row>
+    <row r="397" spans="1:2">
+      <c r="A397" s="7"/>
+      <c r="B397" s="7"/>
+    </row>
+    <row r="398" spans="1:2">
+      <c r="A398" s="7"/>
+      <c r="B398" s="7"/>
+    </row>
+    <row r="399" spans="1:2">
+      <c r="A399" s="7"/>
+      <c r="B399" s="7"/>
+    </row>
+    <row r="400" spans="1:2">
+      <c r="A400" s="7"/>
+      <c r="B400" s="7"/>
+    </row>
+    <row r="401" spans="1:2">
+      <c r="A401" s="7"/>
+      <c r="B401" s="7"/>
+    </row>
+    <row r="402" spans="1:2">
+      <c r="A402" s="7"/>
+      <c r="B402" s="7"/>
+    </row>
+    <row r="403" spans="1:2">
+      <c r="A403" s="7"/>
+      <c r="B403" s="7"/>
+    </row>
+    <row r="404" spans="1:2">
+      <c r="A404" s="7"/>
+      <c r="B404" s="7"/>
+    </row>
+    <row r="405" spans="1:2">
+      <c r="A405" s="7"/>
+      <c r="B405" s="7"/>
+    </row>
+    <row r="406" spans="1:2">
+      <c r="A406" s="7"/>
+      <c r="B406" s="7"/>
+    </row>
+    <row r="407" spans="1:2">
+      <c r="A407" s="7"/>
+      <c r="B407" s="7"/>
+    </row>
+    <row r="408" spans="1:2">
+      <c r="A408" s="7"/>
+      <c r="B408" s="7"/>
+    </row>
+    <row r="409" spans="1:2">
+      <c r="A409" s="7"/>
+      <c r="B409" s="7"/>
+    </row>
+    <row r="410" spans="1:2">
+      <c r="A410" s="7"/>
+      <c r="B410" s="7"/>
+    </row>
+    <row r="411" spans="1:2">
+      <c r="A411" s="7"/>
+      <c r="B411" s="7"/>
+    </row>
+    <row r="412" spans="1:2">
+      <c r="A412" s="7"/>
+      <c r="B412" s="7"/>
+    </row>
+    <row r="413" spans="1:2">
+      <c r="A413" s="7"/>
+      <c r="B413" s="7"/>
+    </row>
+    <row r="414" spans="1:2">
+      <c r="A414" s="7"/>
+      <c r="B414" s="7"/>
+    </row>
+    <row r="415" spans="1:2">
+      <c r="A415" s="7"/>
+      <c r="B415" s="7"/>
+    </row>
+    <row r="416" spans="1:2">
+      <c r="A416" s="7"/>
+      <c r="B416" s="7"/>
+    </row>
+    <row r="417" spans="1:2">
+      <c r="A417" s="7"/>
+      <c r="B417" s="7"/>
+    </row>
+    <row r="418" spans="1:2">
+      <c r="A418" s="7"/>
+      <c r="B418" s="7"/>
+    </row>
+    <row r="419" spans="1:2">
+      <c r="A419" s="7"/>
+      <c r="B419" s="7"/>
+    </row>
+    <row r="420" spans="1:2">
+      <c r="A420" s="7"/>
+      <c r="B420" s="7"/>
+    </row>
+    <row r="421" spans="1:2">
+      <c r="A421" s="7"/>
+      <c r="B421" s="7"/>
+    </row>
+    <row r="422" spans="1:2">
+      <c r="A422" s="7"/>
+      <c r="B422" s="7"/>
+    </row>
+    <row r="423" spans="1:2">
+      <c r="A423" s="7"/>
+      <c r="B423" s="7"/>
+    </row>
+    <row r="424" spans="1:2">
+      <c r="A424" s="7"/>
+      <c r="B424" s="7"/>
+    </row>
+    <row r="425" spans="1:2">
+      <c r="A425" s="7"/>
+      <c r="B425" s="7"/>
+    </row>
+    <row r="426" spans="1:2">
+      <c r="A426" s="7"/>
+      <c r="B426" s="7"/>
+    </row>
+    <row r="427" spans="1:2">
+      <c r="A427" s="7"/>
+      <c r="B427" s="7"/>
+    </row>
+    <row r="428" spans="1:2">
+      <c r="A428" s="7"/>
+      <c r="B428" s="7"/>
+    </row>
+    <row r="429" spans="1:2">
+      <c r="A429" s="7"/>
+      <c r="B429" s="7"/>
+    </row>
+    <row r="430" spans="1:2">
+      <c r="A430" s="7"/>
+      <c r="B430" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>